<commit_message>
add float content and anchor tags
</commit_message>
<xml_diff>
--- a/3pm - web design/web designing attendance.xlsx
+++ b/3pm - web design/web designing attendance.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\11am - krishna sir\3pm - web design\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="120" yWindow="75" windowWidth="19095" windowHeight="11760" activeTab="1"/>
+    <workbookView xWindow="120" yWindow="72" windowWidth="19092" windowHeight="11760" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="11-12" sheetId="1" r:id="rId1"/>
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="197" uniqueCount="81">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="81">
   <si>
     <t>s.no</t>
   </si>
@@ -684,12 +684,12 @@
       <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C2" s="10" t="s">
         <v>26</v>
       </c>
@@ -698,21 +698,21 @@
       <c r="F2" s="11"/>
       <c r="G2" s="11"/>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C3" s="10"/>
       <c r="D3" s="11"/>
       <c r="E3" s="11"/>
       <c r="F3" s="11"/>
       <c r="G3" s="11"/>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:24" x14ac:dyDescent="0.3">
       <c r="C4" s="11"/>
       <c r="D4" s="11"/>
       <c r="E4" s="11"/>
       <c r="F4" s="11"/>
       <c r="G4" s="11"/>
     </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -782,7 +782,7 @@
       <c r="W5" s="3"/>
       <c r="X5" s="3"/>
     </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>1</v>
       </c>
@@ -814,7 +814,7 @@
       <c r="U6" s="1"/>
       <c r="V6" s="1"/>
     </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>2</v>
       </c>
@@ -846,7 +846,7 @@
       <c r="U7" s="1"/>
       <c r="V7" s="1"/>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>3</v>
       </c>
@@ -878,7 +878,7 @@
       <c r="U8" s="1"/>
       <c r="V8" s="1"/>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>4</v>
       </c>
@@ -910,7 +910,7 @@
       <c r="U9" s="1"/>
       <c r="V9" s="1"/>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>5</v>
       </c>
@@ -942,7 +942,7 @@
       <c r="U10" s="1"/>
       <c r="V10" s="1"/>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>6</v>
       </c>
@@ -974,7 +974,7 @@
       <c r="U11" s="1"/>
       <c r="V11" s="1"/>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>7</v>
       </c>
@@ -1006,7 +1006,7 @@
       <c r="U12" s="1"/>
       <c r="V12" s="1"/>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>8</v>
       </c>
@@ -1038,7 +1038,7 @@
       <c r="U13" s="1"/>
       <c r="V13" s="1"/>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>9</v>
       </c>
@@ -1070,7 +1070,7 @@
       <c r="U14" s="1"/>
       <c r="V14" s="1"/>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>10</v>
       </c>
@@ -1102,7 +1102,7 @@
       <c r="U15" s="1"/>
       <c r="V15" s="1"/>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:24" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>11</v>
       </c>
@@ -1134,7 +1134,7 @@
       <c r="U16" s="1"/>
       <c r="V16" s="1"/>
     </row>
-    <row r="17" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>12</v>
       </c>
@@ -1166,7 +1166,7 @@
       <c r="U17" s="1"/>
       <c r="V17" s="1"/>
     </row>
-    <row r="18" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>13</v>
       </c>
@@ -1198,7 +1198,7 @@
       <c r="U18" s="1"/>
       <c r="V18" s="1"/>
     </row>
-    <row r="19" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>14</v>
       </c>
@@ -1230,7 +1230,7 @@
       <c r="U19" s="1"/>
       <c r="V19" s="1"/>
     </row>
-    <row r="20" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>15</v>
       </c>
@@ -1262,7 +1262,7 @@
       <c r="U20" s="1"/>
       <c r="V20" s="1"/>
     </row>
-    <row r="21" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>16</v>
       </c>
@@ -1294,7 +1294,7 @@
       <c r="U21" s="1"/>
       <c r="V21" s="1"/>
     </row>
-    <row r="22" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>17</v>
       </c>
@@ -1326,7 +1326,7 @@
       <c r="U22" s="1"/>
       <c r="V22" s="1"/>
     </row>
-    <row r="23" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>18</v>
       </c>
@@ -1358,7 +1358,7 @@
       <c r="U23" s="1"/>
       <c r="V23" s="1"/>
     </row>
-    <row r="24" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>19</v>
       </c>
@@ -1390,7 +1390,7 @@
       <c r="U24" s="1"/>
       <c r="V24" s="1"/>
     </row>
-    <row r="25" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>20</v>
       </c>
@@ -1422,7 +1422,7 @@
       <c r="U25" s="1"/>
       <c r="V25" s="1"/>
     </row>
-    <row r="26" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>21</v>
       </c>
@@ -1454,7 +1454,7 @@
       <c r="U26" s="1"/>
       <c r="V26" s="1"/>
     </row>
-    <row r="27" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>22</v>
       </c>
@@ -1486,7 +1486,7 @@
       <c r="U27" s="1"/>
       <c r="V27" s="1"/>
     </row>
-    <row r="28" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>23</v>
       </c>
@@ -1518,7 +1518,7 @@
       <c r="U28" s="1"/>
       <c r="V28" s="1"/>
     </row>
-    <row r="29" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>24</v>
       </c>
@@ -1550,7 +1550,7 @@
       <c r="U29" s="1"/>
       <c r="V29" s="1"/>
     </row>
-    <row r="30" spans="1:22" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A30" s="5">
         <v>25</v>
       </c>
@@ -1577,30 +1577,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:W30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="E31" sqref="E31"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="23.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:23" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:23" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="C2" s="4"/>
       <c r="D2" s="7" t="s">
         <v>80</v>
       </c>
       <c r="E2" s="4"/>
     </row>
-    <row r="3" spans="1:23" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:23" ht="20.399999999999999" x14ac:dyDescent="0.35">
       <c r="C3" s="12" t="s">
         <v>47</v>
       </c>
       <c r="D3" s="12"/>
       <c r="E3" s="12"/>
     </row>
-    <row r="5" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
         <v>0</v>
       </c>
@@ -1669,7 +1669,7 @@
       </c>
       <c r="W5" s="3"/>
     </row>
-    <row r="6" spans="1:23" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>1</v>
       </c>
@@ -1682,8 +1682,11 @@
       <c r="D6" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="7" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>2</v>
       </c>
@@ -1696,8 +1699,11 @@
       <c r="D7" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="8" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E7" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>3</v>
       </c>
@@ -1710,8 +1716,11 @@
       <c r="D8" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="9" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E8" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>4</v>
       </c>
@@ -1724,8 +1733,11 @@
       <c r="D9" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="10" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E9" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>5</v>
       </c>
@@ -1738,8 +1750,11 @@
       <c r="D10" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="11" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E10" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>6</v>
       </c>
@@ -1752,8 +1767,11 @@
       <c r="D11" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="12" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>7</v>
       </c>
@@ -1766,8 +1784,11 @@
       <c r="D12" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="13" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E12" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>8</v>
       </c>
@@ -1780,8 +1801,11 @@
       <c r="D13" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="14" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E13" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>9</v>
       </c>
@@ -1794,8 +1818,11 @@
       <c r="D14" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="15" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E14" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>10</v>
       </c>
@@ -1808,8 +1835,11 @@
       <c r="D15" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="16" spans="1:23" x14ac:dyDescent="0.25">
+      <c r="E15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>11</v>
       </c>
@@ -1822,8 +1852,11 @@
       <c r="D16" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E16" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>12</v>
       </c>
@@ -1836,8 +1869,11 @@
       <c r="D17" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E17" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>13</v>
       </c>
@@ -1850,8 +1886,11 @@
       <c r="D18" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E18" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>14</v>
       </c>
@@ -1864,8 +1903,11 @@
       <c r="D19" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E19" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>15</v>
       </c>
@@ -1878,8 +1920,11 @@
       <c r="D20" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E20" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>16</v>
       </c>
@@ -1892,8 +1937,11 @@
       <c r="D21" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E21" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>17</v>
       </c>
@@ -1906,8 +1954,11 @@
       <c r="D22" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E22" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>18</v>
       </c>
@@ -1920,8 +1971,11 @@
       <c r="D23" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>19</v>
       </c>
@@ -1934,8 +1988,11 @@
       <c r="D24" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E24" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>20</v>
       </c>
@@ -1948,8 +2005,11 @@
       <c r="D25" t="s">
         <v>73</v>
       </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E25" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>21</v>
       </c>
@@ -1962,8 +2022,11 @@
       <c r="D26" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>22</v>
       </c>
@@ -1976,8 +2039,11 @@
       <c r="D27" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E27" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>23</v>
       </c>
@@ -1990,8 +2056,11 @@
       <c r="D28" t="s">
         <v>75</v>
       </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E28" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>24</v>
       </c>
@@ -2004,8 +2073,11 @@
       <c r="D29" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E29" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>25</v>
       </c>
@@ -2016,6 +2088,9 @@
         <v>73</v>
       </c>
       <c r="D30" t="s">
+        <v>76</v>
+      </c>
+      <c r="E30" t="s">
         <v>76</v>
       </c>
     </row>
@@ -2033,7 +2108,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>